<commit_message>
Final Code for multivariate
- deleted the t+1 shifting
</commit_message>
<xml_diff>
--- a/Multivariate LSTM/France Predictions/ Alsace.xlsx
+++ b/Multivariate LSTM/France Predictions/ Alsace.xlsx
@@ -411,7 +411,7 @@
         <v>2020</v>
       </c>
       <c r="C2">
-        <v>2.628042214214801</v>
+        <v>1.88412460297346</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -428,7 +428,7 @@
         <v>2020</v>
       </c>
       <c r="C3">
-        <v>1.958138704895972</v>
+        <v>2.963985005617141</v>
       </c>
       <c r="D3">
         <v>0.5</v>
@@ -445,7 +445,7 @@
         <v>2020</v>
       </c>
       <c r="C4">
-        <v>3.539830615222453</v>
+        <v>5.690548782646655</v>
       </c>
       <c r="D4">
         <v>0.8660254037844386</v>
@@ -462,7 +462,7 @@
         <v>2020</v>
       </c>
       <c r="C5">
-        <v>6.589260233044623</v>
+        <v>9.67845241189003</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -479,7 +479,7 @@
         <v>2020</v>
       </c>
       <c r="C6">
-        <v>10.48360034286976</v>
+        <v>14.20343604445457</v>
       </c>
       <c r="D6">
         <v>0.8660254037844388</v>
@@ -496,7 +496,7 @@
         <v>2020</v>
       </c>
       <c r="C7">
-        <v>14.69646521568298</v>
+        <v>17.94002422749996</v>
       </c>
       <c r="D7">
         <v>0.5000000000000004</v>
@@ -513,7 +513,7 @@
         <v>2020</v>
       </c>
       <c r="C8">
-        <v>18.3815486228466</v>
+        <v>19.65825523495674</v>
       </c>
       <c r="D8">
         <v>2.220446049250313e-16</v>
@@ -530,7 +530,7 @@
         <v>2020</v>
       </c>
       <c r="C9">
-        <v>20.24391288220882</v>
+        <v>18.6707456177473</v>
       </c>
       <c r="D9">
         <v>-0.4999999999999998</v>
@@ -547,7 +547,7 @@
         <v>2020</v>
       </c>
       <c r="C10">
-        <v>19.48418966889381</v>
+        <v>15.19245520591736</v>
       </c>
       <c r="D10">
         <v>-0.8660254037844385</v>
@@ -564,7 +564,7 @@
         <v>2020</v>
       </c>
       <c r="C11">
-        <v>15.97030569672584</v>
+        <v>10.31735199451446</v>
       </c>
       <c r="D11">
         <v>-1</v>
@@ -581,7 +581,7 @@
         <v>2020</v>
       </c>
       <c r="C12">
-        <v>10.79438072502613</v>
+        <v>5.707128276526927</v>
       </c>
       <c r="D12">
         <v>-0.866025403784439</v>
@@ -598,7 +598,7 @@
         <v>2020</v>
       </c>
       <c r="C13">
-        <v>5.948571594655513</v>
+        <v>2.874920073747634</v>
       </c>
       <c r="D13">
         <v>-0.5000000000000004</v>
@@ -615,7 +615,7 @@
         <v>2021</v>
       </c>
       <c r="C14">
-        <v>2.880151582360267</v>
+        <v>2.044494104981422</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -632,7 +632,7 @@
         <v>2021</v>
       </c>
       <c r="C15">
-        <v>2.175593197941779</v>
+        <v>3.120536034405231</v>
       </c>
       <c r="D15">
         <v>0.5</v>
@@ -649,7 +649,7 @@
         <v>2021</v>
       </c>
       <c r="C16">
-        <v>3.753269975483417</v>
+        <v>5.842496520876884</v>
       </c>
       <c r="D16">
         <v>0.8660254037844386</v>
@@ -666,7 +666,7 @@
         <v>2021</v>
       </c>
       <c r="C17">
-        <v>6.807717143595218</v>
+        <v>9.830776170492172</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -683,7 +683,7 @@
         <v>2021</v>
       </c>
       <c r="C18">
-        <v>10.70682169556618</v>
+        <v>14.34388375043869</v>
       </c>
       <c r="D18">
         <v>0.8660254037844388</v>
@@ -700,7 +700,7 @@
         <v>2021</v>
       </c>
       <c r="C19">
-        <v>14.91763985216618</v>
+        <v>18.07781338751316</v>
       </c>
       <c r="D19">
         <v>0.5000000000000004</v>
@@ -717,7 +717,7 @@
         <v>2021</v>
       </c>
       <c r="C20">
-        <v>18.60405253231525</v>
+        <v>19.74915929794311</v>
       </c>
       <c r="D20">
         <v>2.220446049250313e-16</v>
@@ -734,7 +734,7 @@
         <v>2021</v>
       </c>
       <c r="C21">
-        <v>20.46149666070938</v>
+        <v>18.7635288721323</v>
       </c>
       <c r="D21">
         <v>-0.4999999999999998</v>
@@ -751,7 +751,7 @@
         <v>2021</v>
       </c>
       <c r="C22">
-        <v>19.69011954724789</v>
+        <v>15.28826665341854</v>
       </c>
       <c r="D22">
         <v>-0.8660254037844385</v>
@@ -768,7 +768,7 @@
         <v>2021</v>
       </c>
       <c r="C23">
-        <v>16.19483265042305</v>
+        <v>10.43443363070488</v>
       </c>
       <c r="D23">
         <v>-1</v>
@@ -785,7 +785,7 @@
         <v>2021</v>
       </c>
       <c r="C24">
-        <v>11.01016725361347</v>
+        <v>5.842522013783454</v>
       </c>
       <c r="D24">
         <v>-0.866025403784439</v>
@@ -802,7 +802,7 @@
         <v>2021</v>
       </c>
       <c r="C25">
-        <v>6.153813164532184</v>
+        <v>3.011394528150558</v>
       </c>
       <c r="D25">
         <v>-0.5000000000000004</v>

</xml_diff>